<commit_message>
Fix the software and increment new logic
</commit_message>
<xml_diff>
--- a/Sources/Teste.xlsx
+++ b/Sources/Teste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliasp\Documents\GitHub\python-automatics-data-alterations-in-xml-file\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\python-automatics-data-alterations-in-xml-file\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583DDB66-B862-4F3E-A422-D341124E93AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C1C02D-D9E7-4000-9C00-266CB36C8491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Número da conta</t>
   </si>
@@ -70,16 +70,25 @@
     <t>Valor unitário (novo)</t>
   </si>
   <si>
-    <t>99999917</t>
+    <t>22103808</t>
   </si>
   <si>
-    <t>00111155</t>
+    <t>90303164</t>
   </si>
   <si>
-    <t>22222222</t>
+    <t>78997500</t>
   </si>
   <si>
-    <t>22103808</t>
+    <t>10104020</t>
+  </si>
+  <si>
+    <t>125648978</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -131,20 +140,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -157,12 +153,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -176,6 +170,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -214,6 +217,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -240,14 +244,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -300,61 +297,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}" name="Tabela13" displayName="Tabela13" ref="A1:G2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:G2" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}" name="Tabela13" displayName="Tabela13" ref="A1:G3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:G3" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{AE4A9C64-0A90-4495-BB17-09C0E95CA992}" name="Número da conta" dataDxfId="29" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{30F48DDE-8BF9-46FE-96B7-8374CD8F97C0}" name="Código do procedimento (atual)" dataDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{634D05B9-5FD4-4A33-AC53-5E26A58D8BF6}" name="Código do procedimento (novo)" dataDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{66DFFD62-75DA-40BE-B887-670CE1AC6712}" name="Tipo de tabela (atual)" dataDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{50109550-C17C-498A-8528-426B8B7C2837}" name="Tipo de tabela (novo)" dataDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{CB84EC5B-03C0-46F2-B02B-F8F418302B2E}" name="Unidade de medida (atual)" dataDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{B843398D-0E00-42D0-92BA-AD9ED7F09000}" name="Unidade de medida (novo)" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{AE4A9C64-0A90-4495-BB17-09C0E95CA992}" name="Número da conta" dataDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{30F48DDE-8BF9-46FE-96B7-8374CD8F97C0}" name="Código do procedimento (atual)" dataDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{634D05B9-5FD4-4A33-AC53-5E26A58D8BF6}" name="Código do procedimento (novo)" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{66DFFD62-75DA-40BE-B887-670CE1AC6712}" name="Tipo de tabela (atual)" dataDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{50109550-C17C-498A-8528-426B8B7C2837}" name="Tipo de tabela (novo)" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{CB84EC5B-03C0-46F2-B02B-F8F418302B2E}" name="Unidade de medida (atual)" dataDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{B843398D-0E00-42D0-92BA-AD9ED7F09000}" name="Unidade de medida (novo)" dataDxfId="19" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0F2FB37-2FA7-4ABE-961E-D044033A56E1}" name="Tabela2" displayName="Tabela2" ref="A1:D57" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="A1:D57" xr:uid="{E0F2FB37-2FA7-4ABE-961E-D044033A56E1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}" name="Tabela1343" displayName="Tabela1343" ref="A1:D57" totalsRowShown="0" dataDxfId="4" dataCellStyle="Normal">
+  <autoFilter ref="A1:D57" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C863B0F2-02FC-407C-91A8-E42AD688AA29}" name="Número da conta" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{E268CB74-220B-418C-9C52-BFAF629A6E4C}" name="Código de procedimento" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{CE8271B6-8061-48AA-BB99-CFA39A9D5183}" name="Valor unitário (atual)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CA07F3D0-D90B-4DB1-9C5B-C99B2C14FDF5}" name="Valor unitário (novo)" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{ECAD9BC2-67D9-4BCC-B20D-01847AA39423}" name="Número da conta" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{5A930C34-0B87-454D-B5F7-EF7D4828287D}" name="Código de procedimento" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{A92C6306-F9C7-4B61-9058-7A1C4913D93E}" name="Valor unitário (atual)" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{4BC2872E-742C-4072-B1B2-ABFAC3B029C0}" name="Valor unitário (novo)" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:G5" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="10" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:G3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:G3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}"/>
-  <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código do procedimento (atual)" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Código do procedimento (novo)" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Tipo de tabela (atual)" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{F28D723F-22B3-48E5-9EAE-B494CB7B6E6E}" name="Tipo de tabela (novo)" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{5D954E41-8139-4FF1-99BA-5DD4542C3385}" name="Unidade de medida (atual)" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{4BD77B0E-1BC3-4C46-801E-E0C3BD669F31}" name="Unidade de medida (novo)" dataDxfId="4" dataCellStyle="Normal"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="9" dataCellStyle="Normal">
+  <autoFilter ref="A1:D57" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}"/>
+  <tableColumns count="4">
+    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="5" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -657,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37037BB9-A3E7-4480-A139-D02AEED3851B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,19 +688,38 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -722,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +763,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>78997500</v>
@@ -778,7 +791,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>90339061</v>
@@ -1396,8 +1409,8 @@
       <c r="A48" s="1">
         <v>22122293</v>
       </c>
-      <c r="B48" s="1">
-        <v>78997500</v>
+      <c r="B48" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C48" s="1">
         <v>0.84</v>
@@ -1522,8 +1535,8 @@
       <c r="A57" s="1">
         <v>22123870</v>
       </c>
-      <c r="B57" s="1">
-        <v>90303164</v>
+      <c r="B57" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C57" s="1">
         <v>0.9</v>
@@ -1533,6 +1546,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1636,62 +1650,816 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16E75D9-ABD9-4040-81D6-B2E7D91186FF}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+      <selection activeCell="C43" sqref="A1:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="4" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>78997500</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>22103808</v>
+      </c>
+      <c r="B3" s="1">
+        <v>90045505</v>
+      </c>
+      <c r="C3" s="1">
+        <v>21.38</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>90339061</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16.22</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B5" s="1">
+        <v>90096924</v>
+      </c>
+      <c r="C5" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>17.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B6" s="1">
+        <v>90378172</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.57</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B7" s="1">
+        <v>90022157</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.52</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B8" s="1">
+        <v>90179994</v>
+      </c>
+      <c r="C8" s="1">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>16.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B9" s="1">
+        <v>79419348</v>
+      </c>
+      <c r="C9" s="1">
+        <v>99</v>
+      </c>
+      <c r="D9" s="1">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B10" s="1">
+        <v>90019830</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B11" s="1">
+        <v>90289870</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>22103878</v>
+      </c>
+      <c r="B12" s="1">
+        <v>90303164</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>22105878</v>
+      </c>
+      <c r="B13" s="1">
+        <v>78997500</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>22107666</v>
+      </c>
+      <c r="B14" s="1">
+        <v>90519515</v>
+      </c>
+      <c r="C14" s="1">
+        <v>27.68</v>
+      </c>
+      <c r="D14" s="1">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>22107666</v>
+      </c>
+      <c r="B15" s="1">
+        <v>78997500</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>22107666</v>
+      </c>
+      <c r="B16" s="1">
+        <v>90257537</v>
+      </c>
+      <c r="C16" s="1">
+        <v>19.32</v>
+      </c>
+      <c r="D16" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B17" s="1">
+        <v>90516532</v>
+      </c>
+      <c r="C17" s="1">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B18" s="1">
+        <v>78997500</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1200329452</v>
+      </c>
+      <c r="C19" s="1">
+        <v>99</v>
+      </c>
+      <c r="D19" s="1">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B20" s="1">
+        <v>90289870</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B21" s="1">
+        <v>90045505</v>
+      </c>
+      <c r="C21" s="1">
+        <v>21.38</v>
+      </c>
+      <c r="D21" s="1">
+        <v>19.34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B22" s="1">
+        <v>90122941</v>
+      </c>
+      <c r="C22" s="1">
+        <v>69.06</v>
+      </c>
+      <c r="D22" s="1">
+        <v>66.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B23" s="1">
+        <v>90395972</v>
+      </c>
+      <c r="C23" s="1">
+        <v>9.16</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22111440</v>
+      </c>
+      <c r="B24" s="1">
+        <v>90486323</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10.95</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10.51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>22117478</v>
+      </c>
+      <c r="B25" s="1">
+        <v>90096924</v>
+      </c>
+      <c r="C25" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="D25" s="1">
+        <v>17.09</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>22117478</v>
+      </c>
+      <c r="B26" s="1">
+        <v>90461185</v>
+      </c>
+      <c r="C26" s="1">
+        <v>102.9</v>
+      </c>
+      <c r="D26" s="1">
+        <v>98.79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>22117478</v>
+      </c>
+      <c r="B27" s="1">
+        <v>90372310</v>
+      </c>
+      <c r="C27" s="1">
+        <v>10.81</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10.39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>22117478</v>
+      </c>
+      <c r="B28" s="1">
+        <v>90433262</v>
+      </c>
+      <c r="C28" s="1">
+        <v>56.72</v>
+      </c>
+      <c r="D28" s="1">
+        <v>54.46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>22117478</v>
+      </c>
+      <c r="B29" s="1">
+        <v>79419348</v>
+      </c>
+      <c r="C29" s="1">
+        <v>99</v>
+      </c>
+      <c r="D29" s="1">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>22117478</v>
+      </c>
+      <c r="B30" s="1">
+        <v>90289870</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>22118566</v>
+      </c>
+      <c r="B31" s="1">
+        <v>90257537</v>
+      </c>
+      <c r="C31" s="1">
+        <v>19.32</v>
+      </c>
+      <c r="D31" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>22118566</v>
+      </c>
+      <c r="B32" s="1">
+        <v>90374959</v>
+      </c>
+      <c r="C32" s="1">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="D32" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B33" s="1">
+        <v>90185048</v>
+      </c>
+      <c r="C33" s="1">
+        <v>95.5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>91.68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B34" s="1">
+        <v>90103017</v>
+      </c>
+      <c r="C34" s="1">
+        <v>658.96</v>
+      </c>
+      <c r="D34" s="1">
+        <v>632.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B35" s="1">
+        <v>90257561</v>
+      </c>
+      <c r="C35" s="1">
+        <v>165.6</v>
+      </c>
+      <c r="D35" s="1">
+        <v>158.97999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B36" s="1">
+        <v>90516532</v>
+      </c>
+      <c r="C36" s="1">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B37" s="1">
+        <v>90070240</v>
+      </c>
+      <c r="C37" s="1">
+        <v>103.33</v>
+      </c>
+      <c r="D37" s="1">
+        <v>99.21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B38" s="1">
+        <v>90137485</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.38</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B39" s="1">
+        <v>90439139</v>
+      </c>
+      <c r="C39" s="1">
+        <v>187.42</v>
+      </c>
+      <c r="D39" s="1">
+        <v>179.93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B40" s="1">
+        <v>90374959</v>
+      </c>
+      <c r="C40" s="1">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="D40" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B41" s="1">
+        <v>90257537</v>
+      </c>
+      <c r="C41" s="1">
+        <v>19.32</v>
+      </c>
+      <c r="D41" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>22118569</v>
+      </c>
+      <c r="B42" s="1">
+        <v>90222393</v>
+      </c>
+      <c r="C42" s="1">
+        <v>7.91</v>
+      </c>
+      <c r="D42" s="1">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>22121631</v>
+      </c>
+      <c r="B43" s="1">
+        <v>90374959</v>
+      </c>
+      <c r="C43" s="1">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="D43" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>22121631</v>
+      </c>
+      <c r="B44" s="1">
+        <v>90257537</v>
+      </c>
+      <c r="C44" s="1">
+        <v>19.32</v>
+      </c>
+      <c r="D44" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>22121631</v>
+      </c>
+      <c r="B45" s="1">
+        <v>90048580</v>
+      </c>
+      <c r="C45" s="1">
+        <v>20.76</v>
+      </c>
+      <c r="D45" s="1">
+        <v>19.93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>22122065</v>
+      </c>
+      <c r="B46" s="1">
+        <v>78997500</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>22122194</v>
+      </c>
+      <c r="B47" s="1">
+        <v>90257537</v>
+      </c>
+      <c r="C47" s="1">
+        <v>19.32</v>
+      </c>
+      <c r="D47" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>22122293</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>22122293</v>
+      </c>
+      <c r="B49" s="1">
+        <v>90303164</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>22122293</v>
+      </c>
+      <c r="B50" s="1">
+        <v>90031679</v>
+      </c>
+      <c r="C50" s="1">
+        <v>33.15</v>
+      </c>
+      <c r="D50" s="1">
+        <v>31.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>22122616</v>
+      </c>
+      <c r="B51" s="1">
+        <v>90303164</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>22122616</v>
+      </c>
+      <c r="B52" s="1">
+        <v>90019830</v>
+      </c>
+      <c r="C52" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="D52" s="1">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>22123748</v>
+      </c>
+      <c r="B53" s="1">
+        <v>90303164</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>22123748</v>
+      </c>
+      <c r="B54" s="1">
+        <v>90019830</v>
+      </c>
+      <c r="C54" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="D54" s="1">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>22123748</v>
+      </c>
+      <c r="B55" s="1">
+        <v>90032772</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>22123870</v>
+      </c>
+      <c r="B56" s="1">
+        <v>90032772</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>22123870</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.86</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Fix logic when alter procedures
</commit_message>
<xml_diff>
--- a/Sources/Teste.xlsx
+++ b/Sources/Teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\python-automatics-data-alterations-in-xml-file\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C1C02D-D9E7-4000-9C00-266CB36C8491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B2A5B3-16E5-4B65-8694-D8041D3FF18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Número da conta</t>
   </si>
@@ -79,16 +79,25 @@
     <t>78997500</t>
   </si>
   <si>
-    <t>10104020</t>
-  </si>
-  <si>
-    <t>125648978</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>00</t>
+  </si>
+  <si>
+    <t>99999917</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>24,91</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -170,6 +179,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -179,7 +197,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -198,6 +215,32 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -214,40 +257,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -313,10 +322,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}" name="Tabela1343" displayName="Tabela1343" ref="A1:D57" totalsRowShown="0" dataDxfId="4" dataCellStyle="Normal">
-  <autoFilter ref="A1:D57" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}" name="Tabela1343" displayName="Tabela1343" ref="A1:D2" totalsRowShown="0" dataDxfId="18" dataCellStyle="Normal">
+  <autoFilter ref="A1:D2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}"/>
   <tableColumns count="4">
-    <tableColumn id="13" xr3:uid="{ECAD9BC2-67D9-4BCC-B20D-01847AA39423}" name="Número da conta" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{ECAD9BC2-67D9-4BCC-B20D-01847AA39423}" name="Número da conta" dataDxfId="17" dataCellStyle="Normal"/>
     <tableColumn id="1" xr3:uid="{5A930C34-0B87-454D-B5F7-EF7D4828287D}" name="Código de procedimento" dataDxfId="2" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{A92C6306-F9C7-4B61-9058-7A1C4913D93E}" name="Valor unitário (atual)" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{4BC2872E-742C-4072-B1B2-ABFAC3B029C0}" name="Valor unitário (novo)" dataDxfId="0" dataCellStyle="Normal"/>
@@ -326,29 +335,29 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:G5" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="8" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="9" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="7" dataCellStyle="Normal">
   <autoFilter ref="A1:D57" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}"/>
   <tableColumns count="4">
-    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="3" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -654,7 +663,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,36 +699,40 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -733,10 +746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D57"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,787 +775,15 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1">
-        <v>78997500</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>22103808</v>
-      </c>
-      <c r="B3" s="1">
-        <v>90045505</v>
-      </c>
-      <c r="C3" s="1">
-        <v>21.38</v>
-      </c>
-      <c r="D3" s="1">
-        <v>19.34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1">
-        <v>90339061</v>
-      </c>
-      <c r="C4" s="1">
-        <v>16.22</v>
-      </c>
-      <c r="D4" s="1">
-        <v>15.58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B5" s="1">
-        <v>90096924</v>
-      </c>
-      <c r="C5" s="1">
-        <v>17.8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>17.09</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B6" s="1">
-        <v>90378172</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.57</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B7" s="1">
-        <v>90022157</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9.52</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9.14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B8" s="1">
-        <v>90179994</v>
-      </c>
-      <c r="C8" s="1">
-        <v>17.190000000000001</v>
-      </c>
-      <c r="D8" s="1">
-        <v>16.09</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B9" s="1">
-        <v>79419348</v>
-      </c>
-      <c r="C9" s="1">
-        <v>99</v>
-      </c>
-      <c r="D9" s="1">
-        <v>82.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B10" s="1">
-        <v>90019830</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9.25</v>
-      </c>
-      <c r="D10" s="1">
-        <v>8.8800000000000008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B11" s="1">
-        <v>90289870</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.87</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>22103878</v>
-      </c>
-      <c r="B12" s="1">
-        <v>90303164</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>22105878</v>
-      </c>
-      <c r="B13" s="1">
-        <v>78997500</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>22107666</v>
-      </c>
-      <c r="B14" s="1">
-        <v>90519515</v>
-      </c>
-      <c r="C14" s="1">
-        <v>27.68</v>
-      </c>
-      <c r="D14" s="1">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>22107666</v>
-      </c>
-      <c r="B15" s="1">
-        <v>78997500</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>22107666</v>
-      </c>
-      <c r="B16" s="1">
-        <v>90257537</v>
-      </c>
-      <c r="C16" s="1">
-        <v>19.32</v>
-      </c>
-      <c r="D16" s="1">
-        <v>18.55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B17" s="1">
-        <v>90516532</v>
-      </c>
-      <c r="C17" s="1">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1">
-        <v>8.64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B18" s="1">
-        <v>78997500</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1200329452</v>
-      </c>
-      <c r="C19" s="1">
-        <v>99</v>
-      </c>
-      <c r="D19" s="1">
-        <v>82.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B20" s="1">
-        <v>90289870</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.87</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B21" s="1">
-        <v>90045505</v>
-      </c>
-      <c r="C21" s="1">
-        <v>21.38</v>
-      </c>
-      <c r="D21" s="1">
-        <v>19.34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B22" s="1">
-        <v>90122941</v>
-      </c>
-      <c r="C22" s="1">
-        <v>69.06</v>
-      </c>
-      <c r="D22" s="1">
-        <v>66.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B23" s="1">
-        <v>90395972</v>
-      </c>
-      <c r="C23" s="1">
-        <v>9.16</v>
-      </c>
-      <c r="D23" s="1">
-        <v>8.7899999999999991</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22111440</v>
-      </c>
-      <c r="B24" s="1">
-        <v>90486323</v>
-      </c>
-      <c r="C24" s="1">
-        <v>10.95</v>
-      </c>
-      <c r="D24" s="1">
-        <v>10.51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>22117478</v>
-      </c>
-      <c r="B25" s="1">
-        <v>90096924</v>
-      </c>
-      <c r="C25" s="1">
-        <v>17.8</v>
-      </c>
-      <c r="D25" s="1">
-        <v>17.09</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>22117478</v>
-      </c>
-      <c r="B26" s="1">
-        <v>90461185</v>
-      </c>
-      <c r="C26" s="1">
-        <v>102.9</v>
-      </c>
-      <c r="D26" s="1">
-        <v>98.79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>22117478</v>
-      </c>
-      <c r="B27" s="1">
-        <v>90372310</v>
-      </c>
-      <c r="C27" s="1">
-        <v>10.81</v>
-      </c>
-      <c r="D27" s="1">
-        <v>10.39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>22117478</v>
-      </c>
-      <c r="B28" s="1">
-        <v>90433262</v>
-      </c>
-      <c r="C28" s="1">
-        <v>56.72</v>
-      </c>
-      <c r="D28" s="1">
-        <v>54.46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>22117478</v>
-      </c>
-      <c r="B29" s="1">
-        <v>79419348</v>
-      </c>
-      <c r="C29" s="1">
-        <v>99</v>
-      </c>
-      <c r="D29" s="1">
-        <v>82.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>22117478</v>
-      </c>
-      <c r="B30" s="1">
-        <v>90289870</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.87</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>22118566</v>
-      </c>
-      <c r="B31" s="1">
-        <v>90257537</v>
-      </c>
-      <c r="C31" s="1">
-        <v>19.32</v>
-      </c>
-      <c r="D31" s="1">
-        <v>18.55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>22118566</v>
-      </c>
-      <c r="B32" s="1">
-        <v>90374959</v>
-      </c>
-      <c r="C32" s="1">
-        <v>19.010000000000002</v>
-      </c>
-      <c r="D32" s="1">
-        <v>18.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B33" s="1">
-        <v>90185048</v>
-      </c>
-      <c r="C33" s="1">
-        <v>95.5</v>
-      </c>
-      <c r="D33" s="1">
-        <v>91.68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B34" s="1">
-        <v>90103017</v>
-      </c>
-      <c r="C34" s="1">
-        <v>658.96</v>
-      </c>
-      <c r="D34" s="1">
-        <v>632.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B35" s="1">
-        <v>90257561</v>
-      </c>
-      <c r="C35" s="1">
-        <v>165.6</v>
-      </c>
-      <c r="D35" s="1">
-        <v>158.97999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B36" s="1">
-        <v>90516532</v>
-      </c>
-      <c r="C36" s="1">
-        <v>9</v>
-      </c>
-      <c r="D36" s="1">
-        <v>8.64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B37" s="1">
-        <v>90070240</v>
-      </c>
-      <c r="C37" s="1">
-        <v>103.33</v>
-      </c>
-      <c r="D37" s="1">
-        <v>99.21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B38" s="1">
-        <v>90137485</v>
-      </c>
-      <c r="C38" s="1">
-        <v>4.38</v>
-      </c>
-      <c r="D38" s="1">
-        <v>4.22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B39" s="1">
-        <v>90439139</v>
-      </c>
-      <c r="C39" s="1">
-        <v>187.42</v>
-      </c>
-      <c r="D39" s="1">
-        <v>179.93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B40" s="1">
-        <v>90374959</v>
-      </c>
-      <c r="C40" s="1">
-        <v>19.010000000000002</v>
-      </c>
-      <c r="D40" s="1">
-        <v>18.25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B41" s="1">
-        <v>90257537</v>
-      </c>
-      <c r="C41" s="1">
-        <v>19.32</v>
-      </c>
-      <c r="D41" s="1">
-        <v>18.55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>22118569</v>
-      </c>
-      <c r="B42" s="1">
-        <v>90222393</v>
-      </c>
-      <c r="C42" s="1">
-        <v>7.91</v>
-      </c>
-      <c r="D42" s="1">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>22121631</v>
-      </c>
-      <c r="B43" s="1">
-        <v>90374959</v>
-      </c>
-      <c r="C43" s="1">
-        <v>19.010000000000002</v>
-      </c>
-      <c r="D43" s="1">
-        <v>18.25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>22121631</v>
-      </c>
-      <c r="B44" s="1">
-        <v>90257537</v>
-      </c>
-      <c r="C44" s="1">
-        <v>19.32</v>
-      </c>
-      <c r="D44" s="1">
-        <v>18.55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>22121631</v>
-      </c>
-      <c r="B45" s="1">
-        <v>90048580</v>
-      </c>
-      <c r="C45" s="1">
-        <v>20.76</v>
-      </c>
-      <c r="D45" s="1">
-        <v>19.93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>22122065</v>
-      </c>
-      <c r="B46" s="1">
-        <v>78997500</v>
-      </c>
-      <c r="C46" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D46" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>22122194</v>
-      </c>
-      <c r="B47" s="1">
-        <v>90257537</v>
-      </c>
-      <c r="C47" s="1">
-        <v>19.32</v>
-      </c>
-      <c r="D47" s="1">
-        <v>18.55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>22122293</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D48" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>22122293</v>
-      </c>
-      <c r="B49" s="1">
-        <v>90303164</v>
-      </c>
-      <c r="C49" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D49" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>22122293</v>
-      </c>
-      <c r="B50" s="1">
-        <v>90031679</v>
-      </c>
-      <c r="C50" s="1">
-        <v>33.15</v>
-      </c>
-      <c r="D50" s="1">
-        <v>31.82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>22122616</v>
-      </c>
-      <c r="B51" s="1">
-        <v>90303164</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D51" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>22122616</v>
-      </c>
-      <c r="B52" s="1">
-        <v>90019830</v>
-      </c>
-      <c r="C52" s="1">
-        <v>9.25</v>
-      </c>
-      <c r="D52" s="1">
-        <v>8.8800000000000008</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>22123748</v>
-      </c>
-      <c r="B53" s="1">
-        <v>90303164</v>
-      </c>
-      <c r="C53" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D53" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>22123748</v>
-      </c>
-      <c r="B54" s="1">
-        <v>90019830</v>
-      </c>
-      <c r="C54" s="1">
-        <v>9.25</v>
-      </c>
-      <c r="D54" s="1">
-        <v>8.8800000000000008</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>22123748</v>
-      </c>
-      <c r="B55" s="1">
-        <v>90032772</v>
-      </c>
-      <c r="C55" s="1">
-        <v>2.81</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>22123870</v>
-      </c>
-      <c r="B56" s="1">
-        <v>90032772</v>
-      </c>
-      <c r="C56" s="1">
-        <v>2.81</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>22123870</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0.86</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code, fix logic
</commit_message>
<xml_diff>
--- a/Sources/Teste.xlsx
+++ b/Sources/Teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\python-automatics-data-alterations-in-xml-file\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B2A5B3-16E5-4B65-8694-D8041D3FF18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA119EB8-6D4D-4B25-9550-7949536DD425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="690" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Número da conta</t>
   </si>
@@ -94,10 +94,25 @@
     <t>040</t>
   </si>
   <si>
-    <t>24,91</t>
-  </si>
-  <si>
-    <t>25</t>
+    <t>22222222</t>
+  </si>
+  <si>
+    <t>22106869</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11,53</t>
+  </si>
+  <si>
+    <t>12,00</t>
+  </si>
+  <si>
+    <t>asfsaf</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -152,6 +167,10 @@
   <dxfs count="28">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -179,15 +198,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -197,6 +207,41 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -208,36 +253,6 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -326,38 +341,38 @@
   <autoFilter ref="A1:D2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}"/>
   <tableColumns count="4">
     <tableColumn id="13" xr3:uid="{ECAD9BC2-67D9-4BCC-B20D-01847AA39423}" name="Número da conta" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{5A930C34-0B87-454D-B5F7-EF7D4828287D}" name="Código de procedimento" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{A92C6306-F9C7-4B61-9058-7A1C4913D93E}" name="Valor unitário (atual)" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{4BC2872E-742C-4072-B1B2-ABFAC3B029C0}" name="Valor unitário (novo)" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{5A930C34-0B87-454D-B5F7-EF7D4828287D}" name="Código de procedimento" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{A92C6306-F9C7-4B61-9058-7A1C4913D93E}" name="Valor unitário (atual)" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{4BC2872E-742C-4072-B1B2-ABFAC3B029C0}" name="Valor unitário (novo)" dataDxfId="15" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:G5" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="6" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="7" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="5" dataCellStyle="Normal">
   <autoFilter ref="A1:D57" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}"/>
   <tableColumns count="4">
-    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="1" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -662,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37037BB9-A3E7-4480-A139-D02AEED3851B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -697,9 +712,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -716,7 +733,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
@@ -725,7 +744,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -748,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,13 +796,13 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit fixes and finish manual
</commit_message>
<xml_diff>
--- a/Sources/Teste.xlsx
+++ b/Sources/Teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliasp\Documents\GitHub\python-automatics-data-alterations-in-xml-file\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57030CD4-19F8-45A7-835D-9EF389BD09E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267B4CF2-ABDA-4A22-89EB-88DEA3F87215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="0" windowWidth="15405" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Número da conta</t>
   </si>
@@ -94,13 +94,70 @@
     <t>Código de despesa (novo)</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>193,50</t>
-  </si>
-  <si>
-    <t>50000</t>
+    <t>90045505</t>
+  </si>
+  <si>
+    <t>19,34</t>
+  </si>
+  <si>
+    <t>90122941</t>
+  </si>
+  <si>
+    <t>66,30</t>
+  </si>
+  <si>
+    <t>90486323</t>
+  </si>
+  <si>
+    <t>10,51</t>
+  </si>
+  <si>
+    <t>90516532</t>
+  </si>
+  <si>
+    <t>8,64</t>
+  </si>
+  <si>
+    <t>1200288832</t>
+  </si>
+  <si>
+    <t>1200108505</t>
+  </si>
+  <si>
+    <t>98020315</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>79419356</t>
+  </si>
+  <si>
+    <t>1200329452</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>90289870</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>90022181</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -142,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -151,52 +208,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -207,14 +285,34 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -225,6 +323,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -234,41 +333,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -279,10 +343,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -293,6 +353,14 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -315,7 +383,34 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -334,62 +429,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}" name="Tabela13" displayName="Tabela13" ref="A1:K11" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}" name="Tabela13" displayName="Tabela13" ref="A1:K11" totalsRowShown="0" headerRowDxfId="31" dataDxfId="0" headerRowCellStyle="Normal">
   <autoFilter ref="A1:K11" xr:uid="{03C310B8-D564-4A91-9D16-1729C7B6396B}"/>
   <tableColumns count="11">
-    <tableColumn id="13" xr3:uid="{AE4A9C64-0A90-4495-BB17-09C0E95CA992}" name="Número da conta" dataDxfId="29" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{30F48DDE-8BF9-46FE-96B7-8374CD8F97C0}" name="Código do procedimento (atual)" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{634D05B9-5FD4-4A33-AC53-5E26A58D8BF6}" name="Código do procedimento (novo)" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{66DFFD62-75DA-40BE-B887-670CE1AC6712}" name="Tipo de tabela (atual)" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{50109550-C17C-498A-8528-426B8B7C2837}" name="Tipo de tabela (novo)" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{AD385DF5-DEE7-4345-AD8A-D2F4E31A0D76}" name="Grau de participação (atual)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{18F9414F-5C9F-40D7-99C0-EB857E6DFFBC}" name="Grau de participação (novo)" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{216B08B3-F940-4A25-9F29-7286C2179B58}" name="Código de despesa (atual)" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{1C6DC2D0-2B59-4006-8BEF-C01187767746}" name="Código de despesa (novo)" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{CB84EC5B-03C0-46F2-B02B-F8F418302B2E}" name="Unidade de medida (atual)" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{B843398D-0E00-42D0-92BA-AD9ED7F09000}" name="Unidade de medida (novo)" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{AE4A9C64-0A90-4495-BB17-09C0E95CA992}" name="Número da conta" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{30F48DDE-8BF9-46FE-96B7-8374CD8F97C0}" name="Código do procedimento (atual)" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{634D05B9-5FD4-4A33-AC53-5E26A58D8BF6}" name="Código do procedimento (novo)" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{66DFFD62-75DA-40BE-B887-670CE1AC6712}" name="Tipo de tabela (atual)" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{50109550-C17C-498A-8528-426B8B7C2837}" name="Tipo de tabela (novo)" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{AD385DF5-DEE7-4345-AD8A-D2F4E31A0D76}" name="Grau de participação (atual)" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{18F9414F-5C9F-40D7-99C0-EB857E6DFFBC}" name="Grau de participação (novo)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{216B08B3-F940-4A25-9F29-7286C2179B58}" name="Código de despesa (atual)" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{1C6DC2D0-2B59-4006-8BEF-C01187767746}" name="Código de despesa (novo)" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{CB84EC5B-03C0-46F2-B02B-F8F418302B2E}" name="Unidade de medida (atual)" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{B843398D-0E00-42D0-92BA-AD9ED7F09000}" name="Unidade de medida (novo)" dataDxfId="1" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}" name="Tabela1343" displayName="Tabela1343" ref="A1:D2" totalsRowShown="0" dataDxfId="28" dataCellStyle="Normal">
-  <autoFilter ref="A1:D2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}" name="Tabela1343" displayName="Tabela1343" ref="A1:D7" totalsRowShown="0" dataDxfId="16" dataCellStyle="Normal">
+  <autoFilter ref="A1:D7" xr:uid="{1EEBA2B3-2207-4A99-B034-BB8887F18A15}"/>
   <tableColumns count="4">
-    <tableColumn id="13" xr3:uid="{ECAD9BC2-67D9-4BCC-B20D-01847AA39423}" name="Número da conta" dataDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{5A930C34-0B87-454D-B5F7-EF7D4828287D}" name="Código de procedimento" dataDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{A92C6306-F9C7-4B61-9058-7A1C4913D93E}" name="Valor unitário (atual)" dataDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{4BC2872E-742C-4072-B1B2-ABFAC3B029C0}" name="Valor unitário (novo)" dataDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{ECAD9BC2-67D9-4BCC-B20D-01847AA39423}" name="Número da conta" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{5A930C34-0B87-454D-B5F7-EF7D4828287D}" name="Código de procedimento" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{A92C6306-F9C7-4B61-9058-7A1C4913D93E}" name="Valor unitário (atual)" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{4BC2872E-742C-4072-B1B2-ABFAC3B029C0}" name="Valor unitário (novo)" dataDxfId="12" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}" name="Tabela135" displayName="Tabela135" ref="A1:G5" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:G5" xr:uid="{DAD4E4B5-978B-4476-BB28-FD2B8986BB3B}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{730D2E80-696B-49C8-B658-611544BA6B32}" name="Número da conta" dataDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{43D03EEE-D316-4A2B-952D-2AFB9BF1F956}" name="Código do procedimento (atual)" dataDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{D26A90B4-4D2C-4AC9-AAA1-3E0D1906901B}" name="Código do procedimento (novo)" dataDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{123ACA80-9FD5-4E12-A75E-551EB135C67A}" name="Tipo de tabela (atual)" dataDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B5BA2D7D-1AF9-4B1E-B488-92BBF6EF979D}" name="Tipo de tabela (novo)" dataDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{5193FC22-6485-4C68-9021-693085402A1A}" name="Unidade de medida (atual)" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{BE5E29C4-0238-4923-B397-FC264900C3F3}" name="Unidade de medida (novo)" dataDxfId="22" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="14" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}" name="Tabela134" displayName="Tabela134" ref="A1:D57" totalsRowShown="0" dataDxfId="21" dataCellStyle="Normal">
   <autoFilter ref="A1:D57" xr:uid="{51DE6959-D817-4492-B3D4-4658D5AD2B22}"/>
   <tableColumns count="4">
-    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{D82D37B4-934F-41DF-AF84-63D84864C894}" name="Número da conta" dataDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{7D0B944E-87A2-4FEF-B152-E2F7FA2B436F}" name="Código de procedimento" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00FA8051-0576-4CB0-BC28-0A16558FA4FB}" name="Valor unitário (atual)" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{DAA713A3-7DE3-49D7-B733-3E23399D0DD6}" name="Valor unitário (novo)" dataDxfId="17" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -694,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37037BB9-A3E7-4480-A139-D02AEED3851B}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,174 +841,170 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3">
-        <v>1200288832</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1200108505</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3">
-        <v>98020315</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3">
-        <v>79419356</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1200329452</v>
-      </c>
-      <c r="D4" s="3">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3">
-        <v>90289870</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3">
-        <v>36</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3">
-        <v>90022181</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3">
-        <v>36</v>
-      </c>
-      <c r="K6" s="3">
-        <v>4</v>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3">
-        <v>40202615</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>11</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -927,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,15 +1048,63 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5">
+        <v>21.38</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5">
+        <v>69.06</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10.95</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>